<commit_message>
Improve authenticated check. TODO: Modify blancoVueComponent to generate noAuthPath injection code.
</commit_message>
<xml_diff>
--- a/meta/objects/LoginInfo.xlsx
+++ b/meta/objects/LoginInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA9A909-13A3-B64D-95B2-C016FAEF86E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78497FC3-498F-9744-ACE2-1703A1B4CD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30140" windowHeight="18440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>クラス名</t>
   </si>
@@ -1707,7 +1707,7 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1977,7 +1977,9 @@
         <v>31</v>
       </c>
       <c r="B18" s="66"/>
-      <c r="C18" s="67"/>
+      <c r="C18" s="67" t="s">
+        <v>32</v>
+      </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>

</xml_diff>